<commit_message>
Update Remodelled spreadsheet_FINAL Actions_17NOV2021.xlsx
</commit_message>
<xml_diff>
--- a/Remodelled spreadsheet_FINAL Actions_17NOV2021.xlsx
+++ b/Remodelled spreadsheet_FINAL Actions_17NOV2021.xlsx
@@ -13,9 +13,6 @@
     <sheet name="Link to symbol" sheetId="10" r:id="rId4"/>
     <sheet name="Sheet2" sheetId="11" r:id="rId5"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId6"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FINAL!$I$6:$S$135</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'KHOA symbology_Phase 1'!$I$6:$N$55</definedName>
@@ -36,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2186" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2188" uniqueCount="689">
   <si>
     <t>Impact on Portrayal</t>
   </si>
@@ -9430,13 +9427,19 @@
       </rPr>
       <t>(subWG proposed recommendation)</t>
     </r>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>No changes to portrayal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="73" x14ac:knownFonts="1">
+  <fonts count="74" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -9990,6 +9993,15 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="14"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="28">
@@ -11014,7 +11026,7 @@
     <xf numFmtId="0" fontId="65" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="71" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="281">
+  <cellXfs count="285">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -11631,6 +11643,148 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="59" fillId="10" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="27" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="52" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="52" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="9" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="27" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="27" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="9" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="69" fillId="5" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -11652,10 +11806,6 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="53" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="49" fillId="4" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -11665,80 +11815,20 @@
     <xf numFmtId="0" fontId="49" fillId="4" borderId="53" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="9" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="70" fillId="8" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="70" fillId="8" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="10" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="13" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="13" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="13" borderId="53" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -11746,15 +11836,6 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="13" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="13" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="13" borderId="53" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -11764,77 +11845,20 @@
     <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="59" fillId="10" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="27" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="27" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="27" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="73" fillId="15" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="52" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="52" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="8" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="8" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="9" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -11847,7 +11871,7 @@
     <cellStyle name="Neutral 2" xfId="7"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="116">
+  <dxfs count="18">
     <dxf>
       <font>
         <b/>
@@ -11919,630 +11943,6 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF00FF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF00FF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -12765,23 +12165,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Sheet2"/>
-      <sheetName val="Sheet3"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13039,7 +12422,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -13050,10 +12433,10 @@
   <dimension ref="A1:W135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="N9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="M9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="T9" sqref="T9"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13082,18 +12465,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="236" t="s">
+      <c r="F1" s="252" t="s">
         <v>433</v>
       </c>
-      <c r="G1" s="236"/>
+      <c r="G1" s="252"/>
       <c r="H1" s="89"/>
-      <c r="I1" s="227" t="s">
+      <c r="I1" s="243" t="s">
         <v>666</v>
       </c>
-      <c r="J1" s="227"/>
-      <c r="K1" s="227"/>
-      <c r="L1" s="227"/>
-      <c r="M1" s="227"/>
+      <c r="J1" s="243"/>
+      <c r="K1" s="243"/>
+      <c r="L1" s="243"/>
+      <c r="M1" s="243"/>
       <c r="N1" s="201"/>
       <c r="O1" s="198"/>
       <c r="P1" s="198"/>
@@ -13102,22 +12485,22 @@
       <c r="S1" s="200"/>
       <c r="T1" s="200"/>
       <c r="U1" s="201"/>
-      <c r="V1" s="212" t="s">
+      <c r="V1" s="260" t="s">
         <v>668</v>
       </c>
-      <c r="W1" s="212"/>
+      <c r="W1" s="260"/>
     </row>
     <row r="2" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="237" t="s">
+      <c r="F2" s="253" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="238"/>
+      <c r="G2" s="254"/>
       <c r="H2" s="90"/>
-      <c r="I2" s="227"/>
-      <c r="J2" s="227"/>
-      <c r="K2" s="227"/>
-      <c r="L2" s="227"/>
-      <c r="M2" s="227"/>
+      <c r="I2" s="243"/>
+      <c r="J2" s="243"/>
+      <c r="K2" s="243"/>
+      <c r="L2" s="243"/>
+      <c r="M2" s="243"/>
       <c r="N2" s="201"/>
       <c r="O2" s="198"/>
       <c r="P2" s="198"/>
@@ -13126,18 +12509,18 @@
       <c r="S2" s="200"/>
       <c r="T2" s="200"/>
       <c r="U2" s="201"/>
-      <c r="V2" s="212"/>
-      <c r="W2" s="212"/>
+      <c r="V2" s="260"/>
+      <c r="W2" s="260"/>
     </row>
     <row r="3" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F3" s="239"/>
-      <c r="G3" s="240"/>
+      <c r="F3" s="255"/>
+      <c r="G3" s="256"/>
       <c r="H3" s="90"/>
-      <c r="I3" s="227"/>
-      <c r="J3" s="227"/>
-      <c r="K3" s="227"/>
-      <c r="L3" s="227"/>
-      <c r="M3" s="227"/>
+      <c r="I3" s="243"/>
+      <c r="J3" s="243"/>
+      <c r="K3" s="243"/>
+      <c r="L3" s="243"/>
+      <c r="M3" s="243"/>
       <c r="N3" s="201"/>
       <c r="O3" s="198"/>
       <c r="P3" s="198"/>
@@ -13146,20 +12529,20 @@
       <c r="S3" s="200"/>
       <c r="T3" s="200"/>
       <c r="U3" s="201"/>
-      <c r="V3" s="212"/>
-      <c r="W3" s="212"/>
+      <c r="V3" s="260"/>
+      <c r="W3" s="260"/>
     </row>
     <row r="4" spans="1:23" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F4" s="241" t="s">
+      <c r="F4" s="257" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="241"/>
+      <c r="G4" s="257"/>
       <c r="H4" s="94"/>
-      <c r="I4" s="227"/>
-      <c r="J4" s="227"/>
-      <c r="K4" s="227"/>
-      <c r="L4" s="227"/>
-      <c r="M4" s="227"/>
+      <c r="I4" s="243"/>
+      <c r="J4" s="243"/>
+      <c r="K4" s="243"/>
+      <c r="L4" s="243"/>
+      <c r="M4" s="243"/>
       <c r="N4" s="201"/>
       <c r="O4" s="198"/>
       <c r="P4" s="198"/>
@@ -13168,10 +12551,10 @@
       <c r="S4" s="200"/>
       <c r="T4" s="200"/>
       <c r="U4" s="201"/>
-      <c r="V4" s="213" t="s">
+      <c r="V4" s="261" t="s">
         <v>669</v>
       </c>
-      <c r="W4" s="213" t="s">
+      <c r="W4" s="261" t="s">
         <v>670</v>
       </c>
     </row>
@@ -13183,25 +12566,25 @@
         <v>17</v>
       </c>
       <c r="H5" s="94"/>
-      <c r="I5" s="228"/>
-      <c r="J5" s="228"/>
-      <c r="K5" s="228"/>
-      <c r="L5" s="228"/>
-      <c r="M5" s="228"/>
+      <c r="I5" s="244"/>
+      <c r="J5" s="244"/>
+      <c r="K5" s="244"/>
+      <c r="L5" s="244"/>
+      <c r="M5" s="244"/>
       <c r="N5" s="202"/>
       <c r="O5" s="199"/>
-      <c r="P5" s="258" t="s">
+      <c r="P5" s="238" t="s">
         <v>677</v>
       </c>
-      <c r="Q5" s="259"/>
+      <c r="Q5" s="239"/>
       <c r="R5" s="202"/>
-      <c r="S5" s="278" t="s">
+      <c r="S5" s="270" t="s">
         <v>686</v>
       </c>
-      <c r="T5" s="279"/>
+      <c r="T5" s="271"/>
       <c r="U5" s="202"/>
-      <c r="V5" s="214"/>
-      <c r="W5" s="214"/>
+      <c r="V5" s="262"/>
+      <c r="W5" s="262"/>
     </row>
     <row r="6" spans="1:23" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -13237,25 +12620,25 @@
         <v>629</v>
       </c>
       <c r="N6" s="203"/>
-      <c r="O6" s="257" t="s">
+      <c r="O6" s="212" t="s">
         <v>667</v>
       </c>
-      <c r="P6" s="260" t="s">
+      <c r="P6" s="213" t="s">
         <v>671</v>
       </c>
-      <c r="Q6" s="260" t="s">
+      <c r="Q6" s="213" t="s">
         <v>1</v>
       </c>
       <c r="R6" s="203"/>
-      <c r="S6" s="280" t="s">
+      <c r="S6" s="230" t="s">
         <v>685</v>
       </c>
-      <c r="T6" s="280" t="s">
+      <c r="T6" s="230" t="s">
         <v>1</v>
       </c>
       <c r="U6" s="203"/>
-      <c r="V6" s="215"/>
-      <c r="W6" s="215"/>
+      <c r="V6" s="263"/>
+      <c r="W6" s="263"/>
     </row>
     <row r="7" spans="1:23" ht="121.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
@@ -13290,13 +12673,13 @@
         <v>568</v>
       </c>
       <c r="N7" s="204"/>
-      <c r="O7" s="261" t="s">
+      <c r="O7" s="214" t="s">
         <v>630</v>
       </c>
       <c r="P7" s="158" t="s">
         <v>673</v>
       </c>
-      <c r="Q7" s="268"/>
+      <c r="Q7" s="220"/>
       <c r="R7" s="204"/>
       <c r="S7" s="116"/>
       <c r="T7" s="116"/>
@@ -13343,13 +12726,13 @@
         <v>570</v>
       </c>
       <c r="N8" s="205"/>
-      <c r="O8" s="262" t="s">
+      <c r="O8" s="215" t="s">
         <v>661</v>
       </c>
       <c r="P8" s="158" t="s">
         <v>673</v>
       </c>
-      <c r="Q8" s="269"/>
+      <c r="Q8" s="221"/>
       <c r="R8" s="205"/>
       <c r="S8" s="158" t="s">
         <v>24</v>
@@ -13390,13 +12773,13 @@
         <v>568</v>
       </c>
       <c r="N9" s="205"/>
-      <c r="O9" s="262" t="s">
+      <c r="O9" s="215" t="s">
         <v>630</v>
       </c>
       <c r="P9" s="158" t="s">
         <v>673</v>
       </c>
-      <c r="Q9" s="269"/>
+      <c r="Q9" s="221"/>
       <c r="R9" s="205"/>
       <c r="S9" s="85"/>
       <c r="T9" s="85"/>
@@ -13437,13 +12820,13 @@
         <v>569</v>
       </c>
       <c r="N10" s="205"/>
-      <c r="O10" s="262" t="s">
+      <c r="O10" s="215" t="s">
         <v>632</v>
       </c>
       <c r="P10" s="158" t="s">
         <v>673</v>
       </c>
-      <c r="Q10" s="269"/>
+      <c r="Q10" s="221"/>
       <c r="R10" s="205"/>
       <c r="S10" s="85"/>
       <c r="T10" s="85"/>
@@ -13452,7 +12835,7 @@
       <c r="W10" s="85"/>
     </row>
     <row r="11" spans="1:23" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="284" t="s">
         <v>429</v>
       </c>
       <c r="B11" s="46"/>
@@ -13476,25 +12859,29 @@
       <c r="L11" s="10" t="s">
         <v>571</v>
       </c>
-      <c r="M11" s="149" t="s">
+      <c r="M11" s="280" t="s">
         <v>570</v>
       </c>
       <c r="N11" s="205"/>
-      <c r="O11" s="263" t="s">
+      <c r="O11" s="281" t="s">
         <v>631</v>
       </c>
-      <c r="P11" s="158" t="s">
-        <v>673</v>
-      </c>
-      <c r="Q11" s="270" t="s">
+      <c r="P11" s="282" t="s">
+        <v>674</v>
+      </c>
+      <c r="Q11" s="283" t="s">
         <v>680</v>
       </c>
       <c r="R11" s="205"/>
-      <c r="S11" s="85"/>
-      <c r="T11" s="85"/>
+      <c r="S11" s="158" t="s">
+        <v>687</v>
+      </c>
+      <c r="T11" s="158" t="s">
+        <v>688</v>
+      </c>
       <c r="U11" s="205"/>
-      <c r="V11" s="85"/>
-      <c r="W11" s="85"/>
+      <c r="V11" s="103"/>
+      <c r="W11" s="103"/>
     </row>
     <row r="12" spans="1:23" ht="119.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
@@ -13529,13 +12916,13 @@
         <v>568</v>
       </c>
       <c r="N12" s="205"/>
-      <c r="O12" s="262" t="s">
+      <c r="O12" s="215" t="s">
         <v>630</v>
       </c>
       <c r="P12" s="158" t="s">
         <v>673</v>
       </c>
-      <c r="Q12" s="269"/>
+      <c r="Q12" s="221"/>
       <c r="R12" s="205"/>
       <c r="S12" s="85"/>
       <c r="T12" s="85"/>
@@ -13576,13 +12963,13 @@
         <v>570</v>
       </c>
       <c r="N13" s="205"/>
-      <c r="O13" s="262" t="s">
+      <c r="O13" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P13" s="158" t="s">
         <v>672</v>
       </c>
-      <c r="Q13" s="269" t="s">
+      <c r="Q13" s="221" t="s">
         <v>679</v>
       </c>
       <c r="R13" s="205"/>
@@ -13629,13 +13016,13 @@
         <v>568</v>
       </c>
       <c r="N14" s="205"/>
-      <c r="O14" s="262" t="s">
+      <c r="O14" s="215" t="s">
         <v>630</v>
       </c>
       <c r="P14" s="158" t="s">
         <v>673</v>
       </c>
-      <c r="Q14" s="269"/>
+      <c r="Q14" s="221"/>
       <c r="R14" s="205"/>
       <c r="S14" s="85"/>
       <c r="T14" s="85"/>
@@ -13680,13 +13067,13 @@
         <v>579</v>
       </c>
       <c r="N15" s="205"/>
-      <c r="O15" s="262" t="s">
+      <c r="O15" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P15" s="158" t="s">
         <v>672</v>
       </c>
-      <c r="Q15" s="269" t="s">
+      <c r="Q15" s="221" t="s">
         <v>679</v>
       </c>
       <c r="R15" s="205"/>
@@ -13733,13 +13120,13 @@
         <v>568</v>
       </c>
       <c r="N16" s="205"/>
-      <c r="O16" s="262" t="s">
+      <c r="O16" s="215" t="s">
         <v>630</v>
       </c>
       <c r="P16" s="158" t="s">
         <v>673</v>
       </c>
-      <c r="Q16" s="269"/>
+      <c r="Q16" s="221"/>
       <c r="R16" s="205"/>
       <c r="S16" s="85"/>
       <c r="T16" s="85"/>
@@ -13780,13 +13167,13 @@
         <v>610</v>
       </c>
       <c r="N17" s="205"/>
-      <c r="O17" s="262" t="s">
+      <c r="O17" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P17" s="158" t="s">
         <v>678</v>
       </c>
-      <c r="Q17" s="269"/>
+      <c r="Q17" s="221"/>
       <c r="R17" s="205"/>
       <c r="S17" s="85"/>
       <c r="T17" s="85"/>
@@ -13831,13 +13218,13 @@
         <v>611</v>
       </c>
       <c r="N18" s="205"/>
-      <c r="O18" s="262" t="s">
+      <c r="O18" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P18" s="158" t="s">
         <v>672</v>
       </c>
-      <c r="Q18" s="269" t="s">
+      <c r="Q18" s="221" t="s">
         <v>679</v>
       </c>
       <c r="R18" s="205"/>
@@ -13880,13 +13267,13 @@
         <v>610</v>
       </c>
       <c r="N19" s="205"/>
-      <c r="O19" s="262" t="s">
+      <c r="O19" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P19" s="158" t="s">
         <v>678</v>
       </c>
-      <c r="Q19" s="269"/>
+      <c r="Q19" s="221"/>
       <c r="R19" s="205"/>
       <c r="S19" s="85"/>
       <c r="T19" s="85"/>
@@ -13927,13 +13314,13 @@
         <v>610</v>
       </c>
       <c r="N20" s="205"/>
-      <c r="O20" s="262" t="s">
+      <c r="O20" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P20" s="158" t="s">
         <v>678</v>
       </c>
-      <c r="Q20" s="269"/>
+      <c r="Q20" s="221"/>
       <c r="R20" s="205"/>
       <c r="S20" s="85"/>
       <c r="T20" s="85"/>
@@ -13978,13 +13365,13 @@
         <v>570</v>
       </c>
       <c r="N21" s="205"/>
-      <c r="O21" s="262" t="s">
+      <c r="O21" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P21" s="158" t="s">
         <v>678</v>
       </c>
-      <c r="Q21" s="269"/>
+      <c r="Q21" s="221"/>
       <c r="R21" s="205"/>
       <c r="S21" s="85"/>
       <c r="T21" s="85"/>
@@ -14025,13 +13412,13 @@
         <v>610</v>
       </c>
       <c r="N22" s="205"/>
-      <c r="O22" s="262" t="s">
+      <c r="O22" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P22" s="158" t="s">
         <v>676</v>
       </c>
-      <c r="Q22" s="269"/>
+      <c r="Q22" s="221"/>
       <c r="R22" s="205"/>
       <c r="S22" s="85"/>
       <c r="T22" s="85"/>
@@ -14072,13 +13459,13 @@
         <v>570</v>
       </c>
       <c r="N23" s="205"/>
-      <c r="O23" s="262" t="s">
+      <c r="O23" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P23" s="158" t="s">
         <v>672</v>
       </c>
-      <c r="Q23" s="269" t="s">
+      <c r="Q23" s="221" t="s">
         <v>679</v>
       </c>
       <c r="R23" s="205"/>
@@ -14121,13 +13508,13 @@
         <v>610</v>
       </c>
       <c r="N24" s="205"/>
-      <c r="O24" s="262" t="s">
+      <c r="O24" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P24" s="158" t="s">
         <v>678</v>
       </c>
-      <c r="Q24" s="269"/>
+      <c r="Q24" s="221"/>
       <c r="R24" s="205"/>
       <c r="S24" s="85"/>
       <c r="T24" s="85"/>
@@ -14168,13 +13555,13 @@
         <v>610</v>
       </c>
       <c r="N25" s="205"/>
-      <c r="O25" s="262" t="s">
+      <c r="O25" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P25" s="158" t="s">
         <v>678</v>
       </c>
-      <c r="Q25" s="269"/>
+      <c r="Q25" s="221"/>
       <c r="R25" s="205"/>
       <c r="S25" s="85"/>
       <c r="T25" s="85"/>
@@ -14219,13 +13606,13 @@
         <v>574</v>
       </c>
       <c r="N26" s="205"/>
-      <c r="O26" s="262" t="s">
+      <c r="O26" s="215" t="s">
         <v>631</v>
       </c>
       <c r="P26" s="158" t="s">
         <v>673</v>
       </c>
-      <c r="Q26" s="270" t="s">
+      <c r="Q26" s="222" t="s">
         <v>681</v>
       </c>
       <c r="R26" s="205"/>
@@ -14272,13 +13659,13 @@
         <v>578</v>
       </c>
       <c r="N27" s="205"/>
-      <c r="O27" s="262" t="s">
+      <c r="O27" s="215" t="s">
         <v>661</v>
       </c>
       <c r="P27" s="158" t="s">
         <v>673</v>
       </c>
-      <c r="Q27" s="269"/>
+      <c r="Q27" s="221"/>
       <c r="R27" s="205"/>
       <c r="S27" s="85"/>
       <c r="T27" s="85"/>
@@ -14315,13 +13702,13 @@
         <v>586</v>
       </c>
       <c r="N28" s="205"/>
-      <c r="O28" s="262" t="s">
+      <c r="O28" s="215" t="s">
         <v>662</v>
       </c>
       <c r="P28" s="158" t="s">
         <v>673</v>
       </c>
-      <c r="Q28" s="269"/>
+      <c r="Q28" s="221"/>
       <c r="R28" s="205"/>
       <c r="S28" s="85"/>
       <c r="T28" s="85"/>
@@ -14358,13 +13745,13 @@
         <v>587</v>
       </c>
       <c r="N29" s="205"/>
-      <c r="O29" s="262" t="s">
+      <c r="O29" s="215" t="s">
         <v>662</v>
       </c>
       <c r="P29" s="158" t="s">
         <v>673</v>
       </c>
-      <c r="Q29" s="269"/>
+      <c r="Q29" s="221"/>
       <c r="R29" s="205"/>
       <c r="S29" s="85"/>
       <c r="T29" s="85"/>
@@ -14405,7 +13792,7 @@
         <v>580</v>
       </c>
       <c r="P30" s="100"/>
-      <c r="Q30" s="271"/>
+      <c r="Q30" s="223"/>
       <c r="R30" s="205"/>
       <c r="S30" s="159"/>
       <c r="T30" s="85"/>
@@ -14442,13 +13829,13 @@
         <v>574</v>
       </c>
       <c r="N31" s="206"/>
-      <c r="O31" s="262" t="s">
+      <c r="O31" s="215" t="s">
         <v>631</v>
       </c>
       <c r="P31" s="158" t="s">
         <v>673</v>
       </c>
-      <c r="Q31" s="270" t="s">
+      <c r="Q31" s="222" t="s">
         <v>682</v>
       </c>
       <c r="R31" s="206"/>
@@ -14491,13 +13878,13 @@
         <v>568</v>
       </c>
       <c r="N32" s="205"/>
-      <c r="O32" s="262" t="s">
+      <c r="O32" s="215" t="s">
         <v>630</v>
       </c>
       <c r="P32" s="158" t="s">
         <v>673</v>
       </c>
-      <c r="Q32" s="269"/>
+      <c r="Q32" s="221"/>
       <c r="R32" s="205"/>
       <c r="S32" s="85"/>
       <c r="T32" s="85"/>
@@ -14538,13 +13925,13 @@
         <v>568</v>
       </c>
       <c r="N33" s="205"/>
-      <c r="O33" s="262" t="s">
+      <c r="O33" s="215" t="s">
         <v>630</v>
       </c>
       <c r="P33" s="158" t="s">
         <v>673</v>
       </c>
-      <c r="Q33" s="269"/>
+      <c r="Q33" s="221"/>
       <c r="R33" s="205"/>
       <c r="S33" s="85"/>
       <c r="T33" s="85"/>
@@ -14585,13 +13972,13 @@
         <v>582</v>
       </c>
       <c r="N34" s="206"/>
-      <c r="O34" s="264" t="s">
+      <c r="O34" s="216" t="s">
         <v>582</v>
       </c>
       <c r="P34" s="158" t="s">
         <v>675</v>
       </c>
-      <c r="Q34" s="276" t="s">
+      <c r="Q34" s="228" t="s">
         <v>683</v>
       </c>
       <c r="R34" s="206"/>
@@ -14634,11 +14021,11 @@
         <v>610</v>
       </c>
       <c r="N35" s="205"/>
-      <c r="O35" s="262" t="s">
+      <c r="O35" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P35" s="158"/>
-      <c r="Q35" s="269"/>
+      <c r="Q35" s="221"/>
       <c r="R35" s="205"/>
       <c r="S35" s="85"/>
       <c r="T35" s="85"/>
@@ -14679,11 +14066,11 @@
         <v>583</v>
       </c>
       <c r="N36" s="207"/>
-      <c r="O36" s="265" t="s">
+      <c r="O36" s="217" t="s">
         <v>583</v>
       </c>
       <c r="P36" s="147"/>
-      <c r="Q36" s="273"/>
+      <c r="Q36" s="225"/>
       <c r="R36" s="207"/>
       <c r="S36" s="85"/>
       <c r="T36" s="85"/>
@@ -14724,13 +14111,13 @@
         <v>611</v>
       </c>
       <c r="N37" s="205"/>
-      <c r="O37" s="262" t="s">
+      <c r="O37" s="215" t="s">
         <v>661</v>
       </c>
       <c r="P37" s="158" t="s">
         <v>673</v>
       </c>
-      <c r="Q37" s="269"/>
+      <c r="Q37" s="221"/>
       <c r="R37" s="205"/>
       <c r="S37" s="85"/>
       <c r="T37" s="85"/>
@@ -14775,13 +14162,13 @@
         <v>606</v>
       </c>
       <c r="N38" s="205"/>
-      <c r="O38" s="262" t="s">
+      <c r="O38" s="215" t="s">
         <v>665</v>
       </c>
       <c r="P38" s="158" t="s">
         <v>678</v>
       </c>
-      <c r="Q38" s="277" t="s">
+      <c r="Q38" s="229" t="s">
         <v>684</v>
       </c>
       <c r="R38" s="205"/>
@@ -14824,13 +14211,13 @@
         <v>461</v>
       </c>
       <c r="N39" s="205"/>
-      <c r="O39" s="262" t="s">
+      <c r="O39" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P39" s="158" t="s">
         <v>678</v>
       </c>
-      <c r="Q39" s="269"/>
+      <c r="Q39" s="221"/>
       <c r="R39" s="205"/>
       <c r="S39" s="85"/>
       <c r="T39" s="85"/>
@@ -14857,9 +14244,9 @@
       </c>
       <c r="M40" s="102"/>
       <c r="N40" s="205"/>
-      <c r="O40" s="266"/>
+      <c r="O40" s="218"/>
       <c r="P40" s="102"/>
-      <c r="Q40" s="274"/>
+      <c r="Q40" s="226"/>
       <c r="R40" s="205"/>
       <c r="S40" s="103"/>
       <c r="T40" s="85"/>
@@ -14904,7 +14291,7 @@
         <v>580</v>
       </c>
       <c r="P41" s="100"/>
-      <c r="Q41" s="271"/>
+      <c r="Q41" s="223"/>
       <c r="R41" s="205"/>
       <c r="S41" s="159"/>
       <c r="T41" s="85"/>
@@ -14947,13 +14334,13 @@
         <v>570</v>
       </c>
       <c r="N42" s="205"/>
-      <c r="O42" s="262" t="s">
+      <c r="O42" s="215" t="s">
         <v>661</v>
       </c>
       <c r="P42" s="158" t="s">
         <v>673</v>
       </c>
-      <c r="Q42" s="269"/>
+      <c r="Q42" s="221"/>
       <c r="R42" s="205"/>
       <c r="S42" s="85"/>
       <c r="T42" s="85"/>
@@ -15002,7 +14389,7 @@
         <v>580</v>
       </c>
       <c r="P43" s="100"/>
-      <c r="Q43" s="271"/>
+      <c r="Q43" s="223"/>
       <c r="R43" s="205"/>
       <c r="S43" s="159"/>
       <c r="T43" s="85"/>
@@ -15043,13 +14430,13 @@
         <v>610</v>
       </c>
       <c r="N44" s="205"/>
-      <c r="O44" s="262" t="s">
+      <c r="O44" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P44" s="158" t="s">
         <v>678</v>
       </c>
-      <c r="Q44" s="269"/>
+      <c r="Q44" s="221"/>
       <c r="R44" s="205"/>
       <c r="S44" s="85"/>
       <c r="T44" s="85"/>
@@ -15090,11 +14477,11 @@
         <v>594</v>
       </c>
       <c r="N45" s="205"/>
-      <c r="O45" s="262" t="s">
+      <c r="O45" s="215" t="s">
         <v>634</v>
       </c>
       <c r="P45" s="158"/>
-      <c r="Q45" s="269"/>
+      <c r="Q45" s="221"/>
       <c r="R45" s="205"/>
       <c r="S45" s="85"/>
       <c r="T45" s="85"/>
@@ -15139,7 +14526,7 @@
         <v>580</v>
       </c>
       <c r="P46" s="100"/>
-      <c r="Q46" s="271"/>
+      <c r="Q46" s="223"/>
       <c r="R46" s="205"/>
       <c r="S46" s="159"/>
       <c r="T46" s="85"/>
@@ -15180,11 +14567,11 @@
         <v>585</v>
       </c>
       <c r="N47" s="205"/>
-      <c r="O47" s="262" t="s">
+      <c r="O47" s="215" t="s">
         <v>663</v>
       </c>
       <c r="P47" s="158"/>
-      <c r="Q47" s="269"/>
+      <c r="Q47" s="221"/>
       <c r="R47" s="205"/>
       <c r="S47" s="85"/>
       <c r="T47" s="85"/>
@@ -15269,11 +14656,11 @@
         <v>601</v>
       </c>
       <c r="N49" s="205"/>
-      <c r="O49" s="262" t="s">
+      <c r="O49" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P49" s="158"/>
-      <c r="Q49" s="269"/>
+      <c r="Q49" s="221"/>
       <c r="R49" s="205"/>
       <c r="S49" s="85"/>
       <c r="T49" s="85"/>
@@ -15314,11 +14701,11 @@
         <v>610</v>
       </c>
       <c r="N50" s="205"/>
-      <c r="O50" s="262" t="s">
+      <c r="O50" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P50" s="158"/>
-      <c r="Q50" s="269"/>
+      <c r="Q50" s="221"/>
       <c r="R50" s="205"/>
       <c r="S50" s="85"/>
       <c r="T50" s="85"/>
@@ -15363,11 +14750,11 @@
         <v>612</v>
       </c>
       <c r="N51" s="205"/>
-      <c r="O51" s="262" t="s">
+      <c r="O51" s="215" t="s">
         <v>631</v>
       </c>
       <c r="P51" s="158"/>
-      <c r="Q51" s="269"/>
+      <c r="Q51" s="221"/>
       <c r="R51" s="205"/>
       <c r="S51" s="85"/>
       <c r="T51" s="85"/>
@@ -15408,11 +14795,11 @@
         <v>613</v>
       </c>
       <c r="N52" s="205"/>
-      <c r="O52" s="262" t="s">
+      <c r="O52" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P52" s="158"/>
-      <c r="Q52" s="269"/>
+      <c r="Q52" s="221"/>
       <c r="R52" s="205"/>
       <c r="S52" s="85"/>
       <c r="T52" s="85"/>
@@ -15459,11 +14846,11 @@
         <v>588</v>
       </c>
       <c r="N53" s="205"/>
-      <c r="O53" s="262" t="s">
+      <c r="O53" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P53" s="158"/>
-      <c r="Q53" s="269"/>
+      <c r="Q53" s="221"/>
       <c r="R53" s="205"/>
       <c r="S53" s="85"/>
       <c r="T53" s="85"/>
@@ -15504,11 +14891,11 @@
         <v>605</v>
       </c>
       <c r="N54" s="205"/>
-      <c r="O54" s="262" t="s">
+      <c r="O54" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P54" s="158"/>
-      <c r="Q54" s="269"/>
+      <c r="Q54" s="221"/>
       <c r="R54" s="205"/>
       <c r="S54" s="85"/>
       <c r="T54" s="85"/>
@@ -15549,11 +14936,11 @@
         <v>581</v>
       </c>
       <c r="N55" s="206"/>
-      <c r="O55" s="264" t="s">
+      <c r="O55" s="216" t="s">
         <v>581</v>
       </c>
       <c r="P55" s="147"/>
-      <c r="Q55" s="272"/>
+      <c r="Q55" s="224"/>
       <c r="R55" s="206"/>
       <c r="S55" s="85"/>
       <c r="T55" s="85"/>
@@ -15594,11 +14981,11 @@
         <v>610</v>
       </c>
       <c r="N56" s="205"/>
-      <c r="O56" s="262" t="s">
+      <c r="O56" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P56" s="158"/>
-      <c r="Q56" s="269"/>
+      <c r="Q56" s="221"/>
       <c r="R56" s="205"/>
       <c r="S56" s="85"/>
       <c r="T56" s="85"/>
@@ -15639,11 +15026,11 @@
         <v>610</v>
       </c>
       <c r="N57" s="205"/>
-      <c r="O57" s="262" t="s">
+      <c r="O57" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P57" s="158"/>
-      <c r="Q57" s="269"/>
+      <c r="Q57" s="221"/>
       <c r="R57" s="205"/>
       <c r="S57" s="85"/>
       <c r="T57" s="85"/>
@@ -15688,11 +15075,11 @@
         <v>589</v>
       </c>
       <c r="N58" s="205"/>
-      <c r="O58" s="262" t="s">
+      <c r="O58" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P58" s="158"/>
-      <c r="Q58" s="269"/>
+      <c r="Q58" s="221"/>
       <c r="R58" s="205"/>
       <c r="S58" s="85"/>
       <c r="T58" s="85"/>
@@ -15733,11 +15120,11 @@
         <v>581</v>
       </c>
       <c r="N59" s="206"/>
-      <c r="O59" s="264" t="s">
+      <c r="O59" s="216" t="s">
         <v>581</v>
       </c>
       <c r="P59" s="147"/>
-      <c r="Q59" s="272"/>
+      <c r="Q59" s="224"/>
       <c r="R59" s="206"/>
       <c r="S59" s="85"/>
       <c r="T59" s="85"/>
@@ -15778,11 +15165,11 @@
         <v>591</v>
       </c>
       <c r="N60" s="205"/>
-      <c r="O60" s="262" t="s">
+      <c r="O60" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P60" s="158"/>
-      <c r="Q60" s="269"/>
+      <c r="Q60" s="221"/>
       <c r="R60" s="205"/>
       <c r="S60" s="85"/>
       <c r="T60" s="85"/>
@@ -15827,11 +15214,11 @@
         <v>568</v>
       </c>
       <c r="N61" s="205"/>
-      <c r="O61" s="262" t="s">
+      <c r="O61" s="215" t="s">
         <v>630</v>
       </c>
       <c r="P61" s="158"/>
-      <c r="Q61" s="269"/>
+      <c r="Q61" s="221"/>
       <c r="R61" s="205"/>
       <c r="S61" s="85"/>
       <c r="T61" s="85"/>
@@ -15876,11 +15263,11 @@
         <v>568</v>
       </c>
       <c r="N62" s="205"/>
-      <c r="O62" s="262" t="s">
+      <c r="O62" s="215" t="s">
         <v>630</v>
       </c>
       <c r="P62" s="158"/>
-      <c r="Q62" s="269"/>
+      <c r="Q62" s="221"/>
       <c r="R62" s="205"/>
       <c r="S62" s="85"/>
       <c r="T62" s="85"/>
@@ -15925,11 +15312,11 @@
         <v>612</v>
       </c>
       <c r="N63" s="205"/>
-      <c r="O63" s="262" t="s">
+      <c r="O63" s="215" t="s">
         <v>631</v>
       </c>
       <c r="P63" s="158"/>
-      <c r="Q63" s="269"/>
+      <c r="Q63" s="221"/>
       <c r="R63" s="205"/>
       <c r="S63" s="85"/>
       <c r="T63" s="85"/>
@@ -15970,11 +15357,11 @@
         <v>605</v>
       </c>
       <c r="N64" s="205"/>
-      <c r="O64" s="262" t="s">
+      <c r="O64" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P64" s="158"/>
-      <c r="Q64" s="269"/>
+      <c r="Q64" s="221"/>
       <c r="R64" s="205"/>
       <c r="S64" s="85"/>
       <c r="T64" s="85"/>
@@ -15994,10 +15381,10 @@
       <c r="E65" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="F65" s="229" t="s">
+      <c r="F65" s="245" t="s">
         <v>229</v>
       </c>
-      <c r="G65" s="230"/>
+      <c r="G65" s="246"/>
       <c r="H65" s="93"/>
       <c r="I65" s="111"/>
       <c r="J65" s="101" t="s">
@@ -16013,11 +15400,11 @@
         <v>619</v>
       </c>
       <c r="N65" s="205"/>
-      <c r="O65" s="262" t="s">
+      <c r="O65" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P65" s="158"/>
-      <c r="Q65" s="269"/>
+      <c r="Q65" s="221"/>
       <c r="R65" s="205"/>
       <c r="S65" s="85"/>
       <c r="T65" s="85"/>
@@ -16058,11 +15445,11 @@
         <v>581</v>
       </c>
       <c r="N66" s="206"/>
-      <c r="O66" s="264" t="s">
+      <c r="O66" s="216" t="s">
         <v>581</v>
       </c>
-      <c r="P66" s="272"/>
-      <c r="Q66" s="272"/>
+      <c r="P66" s="224"/>
+      <c r="Q66" s="224"/>
       <c r="R66" s="206"/>
       <c r="S66" s="85"/>
       <c r="T66" s="85"/>
@@ -16082,10 +15469,10 @@
       <c r="E67" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="F67" s="231" t="s">
+      <c r="F67" s="247" t="s">
         <v>235</v>
       </c>
-      <c r="G67" s="232"/>
+      <c r="G67" s="248"/>
       <c r="H67" s="93"/>
       <c r="I67" s="121"/>
       <c r="J67" s="101" t="s">
@@ -16105,7 +15492,7 @@
         <v>580</v>
       </c>
       <c r="P67" s="100"/>
-      <c r="Q67" s="271"/>
+      <c r="Q67" s="223"/>
       <c r="R67" s="205"/>
       <c r="S67" s="159"/>
       <c r="T67" s="85"/>
@@ -16146,11 +15533,11 @@
         <v>620</v>
       </c>
       <c r="N68" s="205"/>
-      <c r="O68" s="262" t="s">
+      <c r="O68" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P68" s="158"/>
-      <c r="Q68" s="269"/>
+      <c r="Q68" s="221"/>
       <c r="R68" s="205"/>
       <c r="S68" s="85"/>
       <c r="T68" s="85"/>
@@ -16195,7 +15582,7 @@
         <v>580</v>
       </c>
       <c r="P69" s="100"/>
-      <c r="Q69" s="271"/>
+      <c r="Q69" s="223"/>
       <c r="R69" s="205"/>
       <c r="S69" s="159"/>
       <c r="T69" s="85"/>
@@ -16240,7 +15627,7 @@
         <v>580</v>
       </c>
       <c r="P70" s="100"/>
-      <c r="Q70" s="271"/>
+      <c r="Q70" s="223"/>
       <c r="R70" s="205"/>
       <c r="S70" s="159"/>
       <c r="T70" s="85"/>
@@ -16285,7 +15672,7 @@
         <v>580</v>
       </c>
       <c r="P71" s="100"/>
-      <c r="Q71" s="271"/>
+      <c r="Q71" s="223"/>
       <c r="R71" s="205"/>
       <c r="S71" s="159"/>
       <c r="T71" s="85"/>
@@ -16305,10 +15692,10 @@
       <c r="E72" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="F72" s="229" t="s">
+      <c r="F72" s="245" t="s">
         <v>229</v>
       </c>
-      <c r="G72" s="230"/>
+      <c r="G72" s="246"/>
       <c r="H72" s="93"/>
       <c r="I72" s="111"/>
       <c r="J72" s="101" t="s">
@@ -16324,11 +15711,11 @@
         <v>617</v>
       </c>
       <c r="N72" s="205"/>
-      <c r="O72" s="262" t="s">
+      <c r="O72" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P72" s="158"/>
-      <c r="Q72" s="269"/>
+      <c r="Q72" s="221"/>
       <c r="R72" s="205"/>
       <c r="S72" s="85"/>
       <c r="T72" s="85"/>
@@ -16369,11 +15756,11 @@
         <v>592</v>
       </c>
       <c r="N73" s="205"/>
-      <c r="O73" s="262" t="s">
+      <c r="O73" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P73" s="158"/>
-      <c r="Q73" s="269"/>
+      <c r="Q73" s="221"/>
       <c r="R73" s="205"/>
       <c r="S73" s="85"/>
       <c r="T73" s="85"/>
@@ -16418,11 +15805,11 @@
         <v>621</v>
       </c>
       <c r="N74" s="205"/>
-      <c r="O74" s="262" t="s">
+      <c r="O74" s="215" t="s">
         <v>661</v>
       </c>
       <c r="P74" s="158"/>
-      <c r="Q74" s="269"/>
+      <c r="Q74" s="221"/>
       <c r="R74" s="205"/>
       <c r="S74" s="85"/>
       <c r="T74" s="85"/>
@@ -16467,7 +15854,7 @@
         <v>580</v>
       </c>
       <c r="P75" s="100"/>
-      <c r="Q75" s="271"/>
+      <c r="Q75" s="223"/>
       <c r="R75" s="205"/>
       <c r="S75" s="159"/>
       <c r="T75" s="85"/>
@@ -16516,7 +15903,7 @@
         <v>580</v>
       </c>
       <c r="P76" s="100"/>
-      <c r="Q76" s="271"/>
+      <c r="Q76" s="223"/>
       <c r="R76" s="205"/>
       <c r="S76" s="159"/>
       <c r="T76" s="85"/>
@@ -16536,10 +15923,10 @@
       <c r="E77" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="F77" s="229" t="s">
+      <c r="F77" s="245" t="s">
         <v>229</v>
       </c>
-      <c r="G77" s="230"/>
+      <c r="G77" s="246"/>
       <c r="H77" s="93"/>
       <c r="I77" s="111"/>
       <c r="J77" s="101" t="s">
@@ -16555,11 +15942,11 @@
         <v>618</v>
       </c>
       <c r="N77" s="205"/>
-      <c r="O77" s="262" t="s">
+      <c r="O77" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P77" s="158"/>
-      <c r="Q77" s="269"/>
+      <c r="Q77" s="221"/>
       <c r="R77" s="205"/>
       <c r="S77" s="85"/>
       <c r="T77" s="85"/>
@@ -16600,11 +15987,11 @@
         <v>605</v>
       </c>
       <c r="N78" s="205"/>
-      <c r="O78" s="262" t="s">
+      <c r="O78" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P78" s="158"/>
-      <c r="Q78" s="269"/>
+      <c r="Q78" s="221"/>
       <c r="R78" s="205"/>
       <c r="S78" s="85"/>
       <c r="T78" s="85"/>
@@ -16645,11 +16032,11 @@
         <v>605</v>
       </c>
       <c r="N79" s="205"/>
-      <c r="O79" s="262" t="s">
+      <c r="O79" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P79" s="158"/>
-      <c r="Q79" s="269"/>
+      <c r="Q79" s="221"/>
       <c r="R79" s="205"/>
       <c r="S79" s="85"/>
       <c r="T79" s="85"/>
@@ -16669,10 +16056,10 @@
       <c r="E80" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="F80" s="229" t="s">
+      <c r="F80" s="245" t="s">
         <v>278</v>
       </c>
-      <c r="G80" s="230"/>
+      <c r="G80" s="246"/>
       <c r="H80" s="93"/>
       <c r="I80" s="111"/>
       <c r="J80" s="99" t="s">
@@ -16692,7 +16079,7 @@
         <v>580</v>
       </c>
       <c r="P80" s="158"/>
-      <c r="Q80" s="271"/>
+      <c r="Q80" s="223"/>
       <c r="R80" s="205"/>
       <c r="S80" s="159"/>
       <c r="T80" s="85"/>
@@ -16733,11 +16120,11 @@
         <v>621</v>
       </c>
       <c r="N81" s="205"/>
-      <c r="O81" s="262" t="s">
+      <c r="O81" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P81" s="158"/>
-      <c r="Q81" s="269"/>
+      <c r="Q81" s="221"/>
       <c r="R81" s="205"/>
       <c r="S81" s="85"/>
       <c r="T81" s="85"/>
@@ -16782,11 +16169,11 @@
         <v>604</v>
       </c>
       <c r="N82" s="205"/>
-      <c r="O82" s="262" t="s">
+      <c r="O82" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P82" s="158"/>
-      <c r="Q82" s="269"/>
+      <c r="Q82" s="221"/>
       <c r="R82" s="205"/>
       <c r="S82" s="85"/>
       <c r="T82" s="85"/>
@@ -16831,7 +16218,7 @@
         <v>580</v>
       </c>
       <c r="P83" s="100"/>
-      <c r="Q83" s="271"/>
+      <c r="Q83" s="223"/>
       <c r="R83" s="205"/>
       <c r="S83" s="159"/>
       <c r="T83" s="85"/>
@@ -16872,11 +16259,11 @@
         <v>621</v>
       </c>
       <c r="N84" s="205"/>
-      <c r="O84" s="262" t="s">
+      <c r="O84" s="215" t="s">
         <v>661</v>
       </c>
       <c r="P84" s="158"/>
-      <c r="Q84" s="269"/>
+      <c r="Q84" s="221"/>
       <c r="R84" s="205"/>
       <c r="S84" s="85"/>
       <c r="T84" s="85"/>
@@ -16919,7 +16306,7 @@
         <v>580</v>
       </c>
       <c r="P85" s="100"/>
-      <c r="Q85" s="271"/>
+      <c r="Q85" s="223"/>
       <c r="R85" s="205"/>
       <c r="S85" s="159"/>
       <c r="T85" s="85"/>
@@ -16960,11 +16347,11 @@
         <v>605</v>
       </c>
       <c r="N86" s="205"/>
-      <c r="O86" s="262" t="s">
+      <c r="O86" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P86" s="158"/>
-      <c r="Q86" s="269"/>
+      <c r="Q86" s="221"/>
       <c r="R86" s="205"/>
       <c r="S86" s="85"/>
       <c r="T86" s="85"/>
@@ -17005,11 +16392,11 @@
         <v>605</v>
       </c>
       <c r="N87" s="205"/>
-      <c r="O87" s="262" t="s">
+      <c r="O87" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P87" s="158"/>
-      <c r="Q87" s="269"/>
+      <c r="Q87" s="221"/>
       <c r="R87" s="205"/>
       <c r="S87" s="85"/>
       <c r="T87" s="85"/>
@@ -17050,11 +16437,11 @@
         <v>605</v>
       </c>
       <c r="N88" s="205"/>
-      <c r="O88" s="262" t="s">
+      <c r="O88" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P88" s="158"/>
-      <c r="Q88" s="269"/>
+      <c r="Q88" s="221"/>
       <c r="R88" s="205"/>
       <c r="S88" s="85"/>
       <c r="T88" s="85"/>
@@ -17095,11 +16482,11 @@
         <v>593</v>
       </c>
       <c r="N89" s="205"/>
-      <c r="O89" s="262" t="s">
+      <c r="O89" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P89" s="158"/>
-      <c r="Q89" s="269"/>
+      <c r="Q89" s="221"/>
       <c r="R89" s="205"/>
       <c r="S89" s="85"/>
       <c r="T89" s="85"/>
@@ -17123,13 +16510,13 @@
       <c r="E90" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="F90" s="229" t="s">
+      <c r="F90" s="245" t="s">
         <v>310</v>
       </c>
-      <c r="G90" s="230"/>
+      <c r="G90" s="246"/>
       <c r="H90" s="97"/>
       <c r="I90" s="111"/>
-      <c r="J90" s="235" t="s">
+      <c r="J90" s="251" t="s">
         <v>311</v>
       </c>
       <c r="K90" s="137" t="s">
@@ -17138,7 +16525,7 @@
       <c r="L90" s="85" t="s">
         <v>558</v>
       </c>
-      <c r="M90" s="242" t="s">
+      <c r="M90" s="258" t="s">
         <v>580</v>
       </c>
       <c r="N90" s="205"/>
@@ -17146,7 +16533,7 @@
         <v>580</v>
       </c>
       <c r="P90" s="100"/>
-      <c r="Q90" s="271"/>
+      <c r="Q90" s="223"/>
       <c r="R90" s="205"/>
       <c r="S90" s="159"/>
       <c r="T90" s="85"/>
@@ -17178,20 +16565,20 @@
       </c>
       <c r="H91" s="97"/>
       <c r="I91" s="111"/>
-      <c r="J91" s="235"/>
+      <c r="J91" s="251"/>
       <c r="K91" s="137" t="s">
         <v>498</v>
       </c>
       <c r="L91" s="85" t="s">
         <v>558</v>
       </c>
-      <c r="M91" s="243"/>
+      <c r="M91" s="259"/>
       <c r="N91" s="205"/>
       <c r="O91" s="111" t="s">
         <v>580</v>
       </c>
       <c r="P91" s="100"/>
-      <c r="Q91" s="271"/>
+      <c r="Q91" s="223"/>
       <c r="R91" s="205"/>
       <c r="S91" s="159"/>
       <c r="T91" s="85"/>
@@ -17232,11 +16619,11 @@
         <v>594</v>
       </c>
       <c r="N92" s="205"/>
-      <c r="O92" s="262" t="s">
+      <c r="O92" s="215" t="s">
         <v>635</v>
       </c>
       <c r="P92" s="158"/>
-      <c r="Q92" s="269"/>
+      <c r="Q92" s="221"/>
       <c r="R92" s="205"/>
       <c r="S92" s="85"/>
       <c r="T92" s="85"/>
@@ -17277,11 +16664,11 @@
         <v>623</v>
       </c>
       <c r="N93" s="205"/>
-      <c r="O93" s="262" t="s">
+      <c r="O93" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P93" s="158"/>
-      <c r="Q93" s="269"/>
+      <c r="Q93" s="221"/>
       <c r="R93" s="205"/>
       <c r="S93" s="85"/>
       <c r="T93" s="85"/>
@@ -17322,11 +16709,11 @@
         <v>624</v>
       </c>
       <c r="N94" s="205"/>
-      <c r="O94" s="262" t="s">
+      <c r="O94" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P94" s="158"/>
-      <c r="Q94" s="269"/>
+      <c r="Q94" s="221"/>
       <c r="R94" s="205"/>
       <c r="S94" s="85"/>
       <c r="T94" s="85"/>
@@ -17371,11 +16758,11 @@
         <v>596</v>
       </c>
       <c r="N95" s="205"/>
-      <c r="O95" s="262" t="s">
+      <c r="O95" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P95" s="158"/>
-      <c r="Q95" s="269"/>
+      <c r="Q95" s="221"/>
       <c r="R95" s="205"/>
       <c r="S95" s="85"/>
       <c r="T95" s="85"/>
@@ -17420,11 +16807,11 @@
         <v>597</v>
       </c>
       <c r="N96" s="205"/>
-      <c r="O96" s="262" t="s">
+      <c r="O96" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P96" s="158"/>
-      <c r="Q96" s="269"/>
+      <c r="Q96" s="221"/>
       <c r="R96" s="205"/>
       <c r="S96" s="85"/>
       <c r="T96" s="85"/>
@@ -17465,11 +16852,11 @@
         <v>605</v>
       </c>
       <c r="N97" s="205"/>
-      <c r="O97" s="262" t="s">
+      <c r="O97" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P97" s="158"/>
-      <c r="Q97" s="269"/>
+      <c r="Q97" s="221"/>
       <c r="R97" s="205"/>
       <c r="S97" s="85"/>
       <c r="T97" s="85"/>
@@ -17514,7 +16901,7 @@
         <v>580</v>
       </c>
       <c r="P98" s="100"/>
-      <c r="Q98" s="271"/>
+      <c r="Q98" s="223"/>
       <c r="R98" s="205"/>
       <c r="S98" s="159"/>
       <c r="T98" s="85"/>
@@ -17559,7 +16946,7 @@
         <v>580</v>
       </c>
       <c r="P99" s="100"/>
-      <c r="Q99" s="271"/>
+      <c r="Q99" s="223"/>
       <c r="R99" s="205"/>
       <c r="S99" s="159"/>
       <c r="T99" s="85"/>
@@ -17600,11 +16987,11 @@
         <v>625</v>
       </c>
       <c r="N100" s="205"/>
-      <c r="O100" s="262" t="s">
+      <c r="O100" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P100" s="158"/>
-      <c r="Q100" s="269"/>
+      <c r="Q100" s="221"/>
       <c r="R100" s="205"/>
       <c r="S100" s="85"/>
       <c r="T100" s="85"/>
@@ -17649,11 +17036,11 @@
         <v>598</v>
       </c>
       <c r="N101" s="205"/>
-      <c r="O101" s="262" t="s">
+      <c r="O101" s="215" t="s">
         <v>632</v>
       </c>
       <c r="P101" s="158"/>
-      <c r="Q101" s="269"/>
+      <c r="Q101" s="221"/>
       <c r="R101" s="205"/>
       <c r="S101" s="85"/>
       <c r="T101" s="85"/>
@@ -17694,11 +17081,11 @@
         <v>625</v>
       </c>
       <c r="N102" s="205"/>
-      <c r="O102" s="262" t="s">
+      <c r="O102" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P102" s="158"/>
-      <c r="Q102" s="269"/>
+      <c r="Q102" s="221"/>
       <c r="R102" s="205"/>
       <c r="S102" s="85"/>
       <c r="T102" s="85"/>
@@ -17722,10 +17109,10 @@
       <c r="E103" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="F103" s="244" t="s">
+      <c r="F103" s="231" t="s">
         <v>235</v>
       </c>
-      <c r="G103" s="245"/>
+      <c r="G103" s="232"/>
       <c r="H103" s="93"/>
       <c r="I103" s="111"/>
       <c r="J103" s="101" t="s">
@@ -17734,7 +17121,7 @@
       <c r="K103" s="122" t="s">
         <v>493</v>
       </c>
-      <c r="L103" s="219" t="s">
+      <c r="L103" s="233" t="s">
         <v>599</v>
       </c>
       <c r="M103" s="100" t="s">
@@ -17745,7 +17132,7 @@
         <v>580</v>
       </c>
       <c r="P103" s="100"/>
-      <c r="Q103" s="271"/>
+      <c r="Q103" s="223"/>
       <c r="R103" s="205"/>
       <c r="S103" s="159"/>
       <c r="T103" s="85"/>
@@ -17783,7 +17170,7 @@
       <c r="K104" s="122" t="s">
         <v>493</v>
       </c>
-      <c r="L104" s="220"/>
+      <c r="L104" s="234"/>
       <c r="M104" s="100" t="s">
         <v>580</v>
       </c>
@@ -17792,7 +17179,7 @@
         <v>580</v>
       </c>
       <c r="P104" s="100"/>
-      <c r="Q104" s="271"/>
+      <c r="Q104" s="223"/>
       <c r="R104" s="205"/>
       <c r="S104" s="159"/>
       <c r="T104" s="85"/>
@@ -17812,10 +17199,10 @@
       <c r="E105" s="8" t="s">
         <v>347</v>
       </c>
-      <c r="F105" s="244" t="s">
+      <c r="F105" s="231" t="s">
         <v>235</v>
       </c>
-      <c r="G105" s="245"/>
+      <c r="G105" s="232"/>
       <c r="H105" s="93"/>
       <c r="I105" s="111"/>
       <c r="J105" s="101" t="s">
@@ -17835,7 +17222,7 @@
         <v>580</v>
       </c>
       <c r="P105" s="100"/>
-      <c r="Q105" s="271"/>
+      <c r="Q105" s="223"/>
       <c r="R105" s="205"/>
       <c r="S105" s="159"/>
       <c r="T105" s="85"/>
@@ -17884,7 +17271,7 @@
         <v>580</v>
       </c>
       <c r="P106" s="100"/>
-      <c r="Q106" s="271"/>
+      <c r="Q106" s="223"/>
       <c r="R106" s="205"/>
       <c r="S106" s="159"/>
       <c r="T106" s="85"/>
@@ -17925,11 +17312,11 @@
         <v>600</v>
       </c>
       <c r="N107" s="205"/>
-      <c r="O107" s="262" t="s">
+      <c r="O107" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P107" s="158"/>
-      <c r="Q107" s="269"/>
+      <c r="Q107" s="221"/>
       <c r="R107" s="205"/>
       <c r="S107" s="85"/>
       <c r="T107" s="85"/>
@@ -17963,18 +17350,18 @@
       <c r="K108" s="122" t="s">
         <v>470</v>
       </c>
-      <c r="L108" s="219" t="s">
+      <c r="L108" s="233" t="s">
         <v>563</v>
       </c>
       <c r="M108" s="151" t="s">
         <v>605</v>
       </c>
       <c r="N108" s="205"/>
-      <c r="O108" s="262" t="s">
+      <c r="O108" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P108" s="158"/>
-      <c r="Q108" s="269"/>
+      <c r="Q108" s="221"/>
       <c r="R108" s="205"/>
       <c r="S108" s="85"/>
       <c r="T108" s="85"/>
@@ -18008,16 +17395,16 @@
       <c r="K109" s="122" t="s">
         <v>470</v>
       </c>
-      <c r="L109" s="220"/>
+      <c r="L109" s="234"/>
       <c r="M109" s="151" t="s">
         <v>605</v>
       </c>
       <c r="N109" s="205"/>
-      <c r="O109" s="262" t="s">
+      <c r="O109" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P109" s="158"/>
-      <c r="Q109" s="269"/>
+      <c r="Q109" s="221"/>
       <c r="R109" s="205"/>
       <c r="S109" s="85"/>
       <c r="T109" s="85"/>
@@ -18058,11 +17445,11 @@
         <v>570</v>
       </c>
       <c r="N110" s="209"/>
-      <c r="O110" s="267" t="s">
+      <c r="O110" s="219" t="s">
         <v>636</v>
       </c>
       <c r="P110" s="158"/>
-      <c r="Q110" s="275"/>
+      <c r="Q110" s="227"/>
       <c r="R110" s="209"/>
       <c r="S110" s="85"/>
       <c r="T110" s="85"/>
@@ -18103,11 +17490,11 @@
         <v>605</v>
       </c>
       <c r="N111" s="205"/>
-      <c r="O111" s="262" t="s">
+      <c r="O111" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P111" s="158"/>
-      <c r="Q111" s="269"/>
+      <c r="Q111" s="221"/>
       <c r="R111" s="205"/>
       <c r="S111" s="85"/>
       <c r="T111" s="85"/>
@@ -18135,24 +17522,24 @@
       </c>
       <c r="H112" s="93"/>
       <c r="I112" s="111"/>
-      <c r="J112" s="235" t="s">
+      <c r="J112" s="251" t="s">
         <v>517</v>
       </c>
-      <c r="K112" s="246" t="s">
+      <c r="K112" s="235" t="s">
         <v>518</v>
       </c>
       <c r="L112" s="143" t="s">
         <v>564</v>
       </c>
-      <c r="M112" s="221" t="s">
+      <c r="M112" s="267" t="s">
         <v>607</v>
       </c>
       <c r="N112" s="205"/>
-      <c r="O112" s="262" t="s">
+      <c r="O112" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P112" s="158"/>
-      <c r="Q112" s="269"/>
+      <c r="Q112" s="221"/>
       <c r="R112" s="205"/>
       <c r="S112" s="85"/>
       <c r="T112" s="85"/>
@@ -18180,18 +17567,18 @@
       </c>
       <c r="H113" s="93"/>
       <c r="I113" s="111"/>
-      <c r="J113" s="235"/>
-      <c r="K113" s="247"/>
+      <c r="J113" s="251"/>
+      <c r="K113" s="236"/>
       <c r="L113" s="143" t="s">
         <v>564</v>
       </c>
-      <c r="M113" s="222"/>
+      <c r="M113" s="268"/>
       <c r="N113" s="205"/>
-      <c r="O113" s="262" t="s">
+      <c r="O113" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P113" s="158"/>
-      <c r="Q113" s="269"/>
+      <c r="Q113" s="221"/>
       <c r="R113" s="205"/>
       <c r="S113" s="85"/>
       <c r="T113" s="85"/>
@@ -18219,18 +17606,18 @@
       </c>
       <c r="H114" s="93"/>
       <c r="I114" s="111"/>
-      <c r="J114" s="235"/>
-      <c r="K114" s="247"/>
+      <c r="J114" s="251"/>
+      <c r="K114" s="236"/>
       <c r="L114" s="143" t="s">
         <v>564</v>
       </c>
-      <c r="M114" s="222"/>
+      <c r="M114" s="268"/>
       <c r="N114" s="205"/>
-      <c r="O114" s="262" t="s">
+      <c r="O114" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P114" s="158"/>
-      <c r="Q114" s="269"/>
+      <c r="Q114" s="221"/>
       <c r="R114" s="205"/>
       <c r="S114" s="85"/>
       <c r="T114" s="85"/>
@@ -18258,18 +17645,18 @@
       </c>
       <c r="H115" s="93"/>
       <c r="I115" s="111"/>
-      <c r="J115" s="235"/>
-      <c r="K115" s="247"/>
+      <c r="J115" s="251"/>
+      <c r="K115" s="236"/>
       <c r="L115" s="143" t="s">
         <v>564</v>
       </c>
-      <c r="M115" s="222"/>
+      <c r="M115" s="268"/>
       <c r="N115" s="205"/>
-      <c r="O115" s="262" t="s">
+      <c r="O115" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P115" s="158"/>
-      <c r="Q115" s="269"/>
+      <c r="Q115" s="221"/>
       <c r="R115" s="205"/>
       <c r="S115" s="85"/>
       <c r="T115" s="85"/>
@@ -18297,18 +17684,18 @@
       </c>
       <c r="H116" s="93"/>
       <c r="I116" s="111"/>
-      <c r="J116" s="235"/>
-      <c r="K116" s="248"/>
+      <c r="J116" s="251"/>
+      <c r="K116" s="237"/>
       <c r="L116" s="143" t="s">
         <v>564</v>
       </c>
-      <c r="M116" s="223"/>
+      <c r="M116" s="269"/>
       <c r="N116" s="205"/>
-      <c r="O116" s="262" t="s">
+      <c r="O116" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P116" s="158"/>
-      <c r="Q116" s="269"/>
+      <c r="Q116" s="221"/>
       <c r="R116" s="205"/>
       <c r="S116" s="85"/>
       <c r="T116" s="85"/>
@@ -18328,10 +17715,10 @@
       <c r="E117" s="66" t="s">
         <v>228</v>
       </c>
-      <c r="F117" s="233" t="s">
+      <c r="F117" s="249" t="s">
         <v>229</v>
       </c>
-      <c r="G117" s="234"/>
+      <c r="G117" s="250"/>
       <c r="H117" s="93"/>
       <c r="I117" s="111"/>
       <c r="J117" s="101" t="s">
@@ -18347,11 +17734,11 @@
         <v>616</v>
       </c>
       <c r="N117" s="205"/>
-      <c r="O117" s="262" t="s">
+      <c r="O117" s="215" t="s">
         <v>635</v>
       </c>
       <c r="P117" s="158"/>
-      <c r="Q117" s="269"/>
+      <c r="Q117" s="221"/>
       <c r="R117" s="205"/>
       <c r="S117" s="85"/>
       <c r="T117" s="85"/>
@@ -18392,11 +17779,11 @@
         <v>626</v>
       </c>
       <c r="N118" s="205"/>
-      <c r="O118" s="262" t="s">
+      <c r="O118" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P118" s="158"/>
-      <c r="Q118" s="269"/>
+      <c r="Q118" s="221"/>
       <c r="R118" s="205"/>
       <c r="S118" s="85"/>
       <c r="T118" s="85"/>
@@ -18441,11 +17828,11 @@
         <v>608</v>
       </c>
       <c r="N119" s="205"/>
-      <c r="O119" s="262" t="s">
+      <c r="O119" s="215" t="s">
         <v>661</v>
       </c>
       <c r="P119" s="158"/>
-      <c r="Q119" s="269"/>
+      <c r="Q119" s="221"/>
       <c r="R119" s="205"/>
       <c r="S119" s="85"/>
       <c r="T119" s="85"/>
@@ -18474,21 +17861,21 @@
       <c r="H120" s="93"/>
       <c r="I120" s="111"/>
       <c r="J120" s="99"/>
-      <c r="K120" s="224" t="s">
+      <c r="K120" s="240" t="s">
         <v>520</v>
       </c>
       <c r="L120" s="101" t="s">
         <v>567</v>
       </c>
-      <c r="M120" s="216" t="s">
+      <c r="M120" s="264" t="s">
         <v>581</v>
       </c>
       <c r="N120" s="206"/>
-      <c r="O120" s="264" t="s">
+      <c r="O120" s="216" t="s">
         <v>581</v>
       </c>
       <c r="P120" s="147"/>
-      <c r="Q120" s="272"/>
+      <c r="Q120" s="224"/>
       <c r="R120" s="206"/>
       <c r="S120" s="85"/>
       <c r="T120" s="85"/>
@@ -18519,17 +17906,17 @@
       <c r="J121" s="101" t="s">
         <v>376</v>
       </c>
-      <c r="K121" s="225"/>
+      <c r="K121" s="241"/>
       <c r="L121" s="101" t="s">
         <v>567</v>
       </c>
-      <c r="M121" s="217"/>
+      <c r="M121" s="265"/>
       <c r="N121" s="206"/>
-      <c r="O121" s="264" t="s">
+      <c r="O121" s="216" t="s">
         <v>581</v>
       </c>
       <c r="P121" s="147"/>
-      <c r="Q121" s="272"/>
+      <c r="Q121" s="224"/>
       <c r="R121" s="206"/>
       <c r="S121" s="85"/>
       <c r="T121" s="85"/>
@@ -18560,17 +17947,17 @@
       <c r="J122" s="101" t="s">
         <v>376</v>
       </c>
-      <c r="K122" s="226"/>
+      <c r="K122" s="242"/>
       <c r="L122" s="101" t="s">
         <v>567</v>
       </c>
-      <c r="M122" s="218"/>
+      <c r="M122" s="266"/>
       <c r="N122" s="206"/>
-      <c r="O122" s="264" t="s">
+      <c r="O122" s="216" t="s">
         <v>581</v>
       </c>
       <c r="P122" s="147"/>
-      <c r="Q122" s="272"/>
+      <c r="Q122" s="224"/>
       <c r="R122" s="206"/>
       <c r="S122" s="85"/>
       <c r="T122" s="85"/>
@@ -18611,11 +17998,11 @@
         <v>626</v>
       </c>
       <c r="N123" s="205"/>
-      <c r="O123" s="262" t="s">
+      <c r="O123" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P123" s="158"/>
-      <c r="Q123" s="269"/>
+      <c r="Q123" s="221"/>
       <c r="R123" s="205"/>
       <c r="S123" s="85"/>
       <c r="T123" s="85"/>
@@ -18660,11 +18047,11 @@
         <v>626</v>
       </c>
       <c r="N124" s="205"/>
-      <c r="O124" s="262" t="s">
+      <c r="O124" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P124" s="158"/>
-      <c r="Q124" s="269"/>
+      <c r="Q124" s="221"/>
       <c r="R124" s="205"/>
       <c r="S124" s="85"/>
       <c r="T124" s="85"/>
@@ -18713,7 +18100,7 @@
         <v>580</v>
       </c>
       <c r="P125" s="100"/>
-      <c r="Q125" s="271"/>
+      <c r="Q125" s="223"/>
       <c r="R125" s="205"/>
       <c r="S125" s="159"/>
       <c r="T125" s="85"/>
@@ -18758,11 +18145,11 @@
         <v>612</v>
       </c>
       <c r="N126" s="205"/>
-      <c r="O126" s="262" t="s">
+      <c r="O126" s="215" t="s">
         <v>631</v>
       </c>
       <c r="P126" s="158"/>
-      <c r="Q126" s="269"/>
+      <c r="Q126" s="221"/>
       <c r="R126" s="205"/>
       <c r="S126" s="85"/>
       <c r="T126" s="85"/>
@@ -18807,11 +18194,11 @@
         <v>609</v>
       </c>
       <c r="N127" s="205"/>
-      <c r="O127" s="262" t="s">
+      <c r="O127" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P127" s="158"/>
-      <c r="Q127" s="269"/>
+      <c r="Q127" s="221"/>
       <c r="R127" s="205"/>
       <c r="S127" s="85"/>
       <c r="T127" s="85"/>
@@ -18856,7 +18243,7 @@
         <v>580</v>
       </c>
       <c r="P128" s="100"/>
-      <c r="Q128" s="271"/>
+      <c r="Q128" s="223"/>
       <c r="R128" s="205"/>
       <c r="S128" s="159"/>
       <c r="T128" s="85"/>
@@ -18897,11 +18284,11 @@
         <v>570</v>
       </c>
       <c r="N129" s="205"/>
-      <c r="O129" s="262" t="s">
+      <c r="O129" s="215" t="s">
         <v>661</v>
       </c>
       <c r="P129" s="158"/>
-      <c r="Q129" s="269"/>
+      <c r="Q129" s="221"/>
       <c r="R129" s="205"/>
       <c r="S129" s="85"/>
       <c r="T129" s="85"/>
@@ -18946,7 +18333,7 @@
         <v>614</v>
       </c>
       <c r="P130" s="158"/>
-      <c r="Q130" s="271"/>
+      <c r="Q130" s="223"/>
       <c r="R130" s="205"/>
       <c r="S130" s="159"/>
       <c r="T130" s="85"/>
@@ -18991,11 +18378,11 @@
         <v>627</v>
       </c>
       <c r="N131" s="205"/>
-      <c r="O131" s="262" t="s">
+      <c r="O131" s="215" t="s">
         <v>630</v>
       </c>
       <c r="P131" s="158"/>
-      <c r="Q131" s="269"/>
+      <c r="Q131" s="221"/>
       <c r="R131" s="205"/>
       <c r="S131" s="85"/>
       <c r="T131" s="85"/>
@@ -19036,11 +18423,11 @@
         <v>628</v>
       </c>
       <c r="N132" s="205"/>
-      <c r="O132" s="262" t="s">
+      <c r="O132" s="215" t="s">
         <v>633</v>
       </c>
       <c r="P132" s="158"/>
-      <c r="Q132" s="269"/>
+      <c r="Q132" s="221"/>
       <c r="R132" s="205"/>
       <c r="S132" s="85"/>
       <c r="T132" s="85"/>
@@ -19081,11 +18468,11 @@
         <v>601</v>
       </c>
       <c r="N133" s="205"/>
-      <c r="O133" s="262" t="s">
+      <c r="O133" s="215" t="s">
         <v>661</v>
       </c>
       <c r="P133" s="158"/>
-      <c r="Q133" s="269"/>
+      <c r="Q133" s="221"/>
       <c r="R133" s="205"/>
       <c r="S133" s="85"/>
       <c r="T133" s="85"/>
@@ -19126,11 +18513,11 @@
         <v>605</v>
       </c>
       <c r="N134" s="205"/>
-      <c r="O134" s="262" t="s">
+      <c r="O134" s="215" t="s">
         <v>664</v>
       </c>
       <c r="P134" s="158"/>
-      <c r="Q134" s="269"/>
+      <c r="Q134" s="221"/>
       <c r="R134" s="205"/>
       <c r="S134" s="85"/>
       <c r="T134" s="85"/>
@@ -19150,10 +18537,10 @@
       <c r="E135" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="F135" s="229" t="s">
+      <c r="F135" s="245" t="s">
         <v>229</v>
       </c>
-      <c r="G135" s="230"/>
+      <c r="G135" s="246"/>
       <c r="H135" s="93"/>
       <c r="I135" s="111"/>
       <c r="J135" s="101" t="s">
@@ -19169,11 +18556,11 @@
         <v>615</v>
       </c>
       <c r="N135" s="205"/>
-      <c r="O135" s="262" t="s">
+      <c r="O135" s="215" t="s">
         <v>635</v>
       </c>
       <c r="P135" s="158"/>
-      <c r="Q135" s="269"/>
+      <c r="Q135" s="221"/>
       <c r="R135" s="205"/>
       <c r="S135" s="85"/>
       <c r="T135" s="85"/>
@@ -19183,11 +18570,13 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="F103:G103"/>
-    <mergeCell ref="F105:G105"/>
-    <mergeCell ref="L103:L104"/>
-    <mergeCell ref="K112:K116"/>
-    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="V1:W3"/>
+    <mergeCell ref="V4:V6"/>
+    <mergeCell ref="W4:W6"/>
+    <mergeCell ref="M120:M122"/>
+    <mergeCell ref="L108:L109"/>
+    <mergeCell ref="M112:M116"/>
+    <mergeCell ref="S5:T5"/>
     <mergeCell ref="K120:K122"/>
     <mergeCell ref="I1:M5"/>
     <mergeCell ref="F135:G135"/>
@@ -19204,13 +18593,11 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="J90:J91"/>
     <mergeCell ref="M90:M91"/>
-    <mergeCell ref="V1:W3"/>
-    <mergeCell ref="V4:V6"/>
-    <mergeCell ref="W4:W6"/>
-    <mergeCell ref="M120:M122"/>
-    <mergeCell ref="L108:L109"/>
-    <mergeCell ref="M112:M116"/>
-    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="F103:G103"/>
+    <mergeCell ref="F105:G105"/>
+    <mergeCell ref="L103:L104"/>
+    <mergeCell ref="K112:K116"/>
+    <mergeCell ref="P5:Q5"/>
   </mergeCells>
   <conditionalFormatting sqref="P7:P29 P37:P54 P56:P58 P60:P65 P123:P135 P32:P35 P67:P119">
     <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
@@ -19322,38 +18709,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="236" t="s">
+      <c r="F1" s="252" t="s">
         <v>433</v>
       </c>
-      <c r="G1" s="236"/>
+      <c r="G1" s="252"/>
       <c r="H1" s="89"/>
-      <c r="I1" s="227" t="s">
+      <c r="I1" s="243" t="s">
         <v>538</v>
       </c>
-      <c r="J1" s="227"/>
-      <c r="K1" s="227"/>
-      <c r="L1" s="227"/>
-      <c r="M1" s="227"/>
-      <c r="N1" s="227"/>
+      <c r="J1" s="243"/>
+      <c r="K1" s="243"/>
+      <c r="L1" s="243"/>
+      <c r="M1" s="243"/>
+      <c r="N1" s="243"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="F2" s="237" t="s">
+      <c r="F2" s="253" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="238"/>
+      <c r="G2" s="254"/>
       <c r="H2" s="90"/>
-      <c r="I2" s="249" t="s">
+      <c r="I2" s="275" t="s">
         <v>434</v>
       </c>
-      <c r="J2" s="250"/>
-      <c r="K2" s="250"/>
-      <c r="L2" s="250"/>
-      <c r="M2" s="250"/>
-      <c r="N2" s="250"/>
+      <c r="J2" s="276"/>
+      <c r="K2" s="276"/>
+      <c r="L2" s="276"/>
+      <c r="M2" s="276"/>
+      <c r="N2" s="276"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="F3" s="239"/>
-      <c r="G3" s="240"/>
+      <c r="F3" s="255"/>
+      <c r="G3" s="256"/>
       <c r="H3" s="90"/>
       <c r="I3" s="82"/>
       <c r="J3" s="82"/>
@@ -19363,10 +18750,10 @@
       <c r="N3" s="81"/>
     </row>
     <row r="4" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F4" s="241" t="s">
+      <c r="F4" s="257" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="241"/>
+      <c r="G4" s="257"/>
       <c r="H4" s="94"/>
       <c r="I4" s="91"/>
       <c r="J4" s="91"/>
@@ -20432,10 +19819,10 @@
       <c r="E37" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="F37" s="229" t="s">
+      <c r="F37" s="245" t="s">
         <v>229</v>
       </c>
-      <c r="G37" s="230"/>
+      <c r="G37" s="246"/>
       <c r="H37" s="93"/>
       <c r="I37" s="111"/>
       <c r="J37" s="101" t="s">
@@ -20496,10 +19883,10 @@
       <c r="E39" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="F39" s="229" t="s">
+      <c r="F39" s="245" t="s">
         <v>229</v>
       </c>
-      <c r="G39" s="230"/>
+      <c r="G39" s="246"/>
       <c r="H39" s="93"/>
       <c r="I39" s="111"/>
       <c r="J39" s="101" t="s">
@@ -20560,10 +19947,10 @@
       <c r="E41" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="F41" s="229" t="s">
+      <c r="F41" s="245" t="s">
         <v>229</v>
       </c>
-      <c r="G41" s="230"/>
+      <c r="G41" s="246"/>
       <c r="H41" s="93"/>
       <c r="I41" s="111"/>
       <c r="J41" s="101" t="s">
@@ -20801,16 +20188,16 @@
       </c>
       <c r="H48" s="93"/>
       <c r="I48" s="111"/>
-      <c r="J48" s="235" t="s">
+      <c r="J48" s="251" t="s">
         <v>517</v>
       </c>
-      <c r="K48" s="246" t="s">
+      <c r="K48" s="235" t="s">
         <v>518</v>
       </c>
       <c r="L48" s="162" t="s">
         <v>564</v>
       </c>
-      <c r="M48" s="251" t="s">
+      <c r="M48" s="272" t="s">
         <v>607</v>
       </c>
       <c r="N48" s="85"/>
@@ -20834,12 +20221,12 @@
       </c>
       <c r="H49" s="93"/>
       <c r="I49" s="111"/>
-      <c r="J49" s="235"/>
-      <c r="K49" s="247"/>
+      <c r="J49" s="251"/>
+      <c r="K49" s="236"/>
       <c r="L49" s="162" t="s">
         <v>564</v>
       </c>
-      <c r="M49" s="252"/>
+      <c r="M49" s="273"/>
       <c r="N49" s="85"/>
     </row>
     <row r="50" spans="2:14" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -20861,12 +20248,12 @@
       </c>
       <c r="H50" s="93"/>
       <c r="I50" s="111"/>
-      <c r="J50" s="235"/>
-      <c r="K50" s="247"/>
+      <c r="J50" s="251"/>
+      <c r="K50" s="236"/>
       <c r="L50" s="162" t="s">
         <v>564</v>
       </c>
-      <c r="M50" s="252"/>
+      <c r="M50" s="273"/>
       <c r="N50" s="85"/>
     </row>
     <row r="51" spans="2:14" ht="43.2" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -20888,12 +20275,12 @@
       </c>
       <c r="H51" s="93"/>
       <c r="I51" s="111"/>
-      <c r="J51" s="235"/>
-      <c r="K51" s="247"/>
+      <c r="J51" s="251"/>
+      <c r="K51" s="236"/>
       <c r="L51" s="162" t="s">
         <v>564</v>
       </c>
-      <c r="M51" s="252"/>
+      <c r="M51" s="273"/>
       <c r="N51" s="85"/>
     </row>
     <row r="52" spans="2:14" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -20915,12 +20302,12 @@
       </c>
       <c r="H52" s="93"/>
       <c r="I52" s="111"/>
-      <c r="J52" s="235"/>
-      <c r="K52" s="248"/>
+      <c r="J52" s="251"/>
+      <c r="K52" s="237"/>
       <c r="L52" s="162" t="s">
         <v>564</v>
       </c>
-      <c r="M52" s="253"/>
+      <c r="M52" s="274"/>
       <c r="N52" s="85"/>
     </row>
     <row r="53" spans="2:14" ht="78" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -20934,10 +20321,10 @@
       <c r="E53" s="66" t="s">
         <v>228</v>
       </c>
-      <c r="F53" s="233" t="s">
+      <c r="F53" s="249" t="s">
         <v>229</v>
       </c>
-      <c r="G53" s="234"/>
+      <c r="G53" s="250"/>
       <c r="H53" s="93"/>
       <c r="I53" s="111"/>
       <c r="J53" s="101" t="s">
@@ -21000,10 +20387,10 @@
       <c r="E55" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="F55" s="229" t="s">
+      <c r="F55" s="245" t="s">
         <v>229</v>
       </c>
-      <c r="G55" s="230"/>
+      <c r="G55" s="246"/>
       <c r="H55" s="93"/>
       <c r="I55" s="111"/>
       <c r="J55" s="101" t="s">
@@ -21487,6 +20874,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="F2:G3"/>
+    <mergeCell ref="F4:G4"/>
     <mergeCell ref="M48:M52"/>
     <mergeCell ref="F55:G55"/>
     <mergeCell ref="F37:G37"/>
@@ -21495,11 +20887,6 @@
     <mergeCell ref="F53:G53"/>
     <mergeCell ref="J48:J52"/>
     <mergeCell ref="K48:K52"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="F2:G3"/>
-    <mergeCell ref="F4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -21529,36 +20916,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="236" t="s">
+      <c r="F1" s="252" t="s">
         <v>433</v>
       </c>
-      <c r="G1" s="236"/>
+      <c r="G1" s="252"/>
       <c r="H1" s="89"/>
-      <c r="I1" s="227" t="s">
+      <c r="I1" s="243" t="s">
         <v>538</v>
       </c>
-      <c r="J1" s="227"/>
-      <c r="K1" s="227"/>
-      <c r="L1" s="227"/>
-      <c r="M1" s="227"/>
+      <c r="J1" s="243"/>
+      <c r="K1" s="243"/>
+      <c r="L1" s="243"/>
+      <c r="M1" s="243"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F2" s="237" t="s">
+      <c r="F2" s="253" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="238"/>
+      <c r="G2" s="254"/>
       <c r="H2" s="90"/>
-      <c r="I2" s="249" t="s">
+      <c r="I2" s="275" t="s">
         <v>434</v>
       </c>
-      <c r="J2" s="250"/>
-      <c r="K2" s="250"/>
-      <c r="L2" s="250"/>
-      <c r="M2" s="250"/>
+      <c r="J2" s="276"/>
+      <c r="K2" s="276"/>
+      <c r="L2" s="276"/>
+      <c r="M2" s="276"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F3" s="239"/>
-      <c r="G3" s="240"/>
+      <c r="F3" s="255"/>
+      <c r="G3" s="256"/>
       <c r="H3" s="90"/>
       <c r="I3" s="82"/>
       <c r="J3" s="82"/>
@@ -21567,10 +20954,10 @@
       <c r="M3" s="82"/>
     </row>
     <row r="4" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F4" s="241" t="s">
+      <c r="F4" s="257" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="241"/>
+      <c r="G4" s="257"/>
       <c r="H4" s="94"/>
       <c r="I4" s="91"/>
       <c r="J4" s="91"/>
@@ -22536,7 +21923,7 @@
       <c r="K32" s="122" t="s">
         <v>470</v>
       </c>
-      <c r="L32" s="254" t="s">
+      <c r="L32" s="277" t="s">
         <v>563</v>
       </c>
       <c r="M32" s="151" t="s">
@@ -22571,7 +21958,7 @@
       <c r="K33" s="122" t="s">
         <v>470</v>
       </c>
-      <c r="L33" s="255"/>
+      <c r="L33" s="278"/>
       <c r="M33" s="151" t="s">
         <v>605</v>
       </c>
@@ -22814,154 +22201,154 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D1" s="256" t="s">
+      <c r="D1" s="279" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="256"/>
-      <c r="F1" s="256"/>
-      <c r="G1" s="256"/>
+      <c r="E1" s="279"/>
+      <c r="F1" s="279"/>
+      <c r="G1" s="279"/>
     </row>
     <row r="2" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D2" s="256"/>
-      <c r="E2" s="256"/>
-      <c r="F2" s="256"/>
-      <c r="G2" s="256"/>
+      <c r="D2" s="279"/>
+      <c r="E2" s="279"/>
+      <c r="F2" s="279"/>
+      <c r="G2" s="279"/>
     </row>
     <row r="3" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D3" s="256"/>
-      <c r="E3" s="256"/>
-      <c r="F3" s="256"/>
-      <c r="G3" s="256"/>
+      <c r="D3" s="279"/>
+      <c r="E3" s="279"/>
+      <c r="F3" s="279"/>
+      <c r="G3" s="279"/>
     </row>
     <row r="4" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D4" s="256"/>
-      <c r="E4" s="256"/>
-      <c r="F4" s="256"/>
-      <c r="G4" s="256"/>
+      <c r="D4" s="279"/>
+      <c r="E4" s="279"/>
+      <c r="F4" s="279"/>
+      <c r="G4" s="279"/>
     </row>
     <row r="5" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D5" s="256"/>
-      <c r="E5" s="256"/>
-      <c r="F5" s="256"/>
-      <c r="G5" s="256"/>
+      <c r="D5" s="279"/>
+      <c r="E5" s="279"/>
+      <c r="F5" s="279"/>
+      <c r="G5" s="279"/>
     </row>
     <row r="6" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D6" s="256"/>
-      <c r="E6" s="256"/>
-      <c r="F6" s="256"/>
-      <c r="G6" s="256"/>
+      <c r="D6" s="279"/>
+      <c r="E6" s="279"/>
+      <c r="F6" s="279"/>
+      <c r="G6" s="279"/>
     </row>
     <row r="7" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D7" s="256"/>
-      <c r="E7" s="256"/>
-      <c r="F7" s="256"/>
-      <c r="G7" s="256"/>
+      <c r="D7" s="279"/>
+      <c r="E7" s="279"/>
+      <c r="F7" s="279"/>
+      <c r="G7" s="279"/>
     </row>
     <row r="8" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D8" s="256"/>
-      <c r="E8" s="256"/>
-      <c r="F8" s="256"/>
-      <c r="G8" s="256"/>
+      <c r="D8" s="279"/>
+      <c r="E8" s="279"/>
+      <c r="F8" s="279"/>
+      <c r="G8" s="279"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="256" t="s">
+      <c r="D12" s="279" t="s">
         <v>659</v>
       </c>
-      <c r="E12" s="256"/>
-      <c r="F12" s="256"/>
-      <c r="G12" s="256"/>
+      <c r="E12" s="279"/>
+      <c r="F12" s="279"/>
+      <c r="G12" s="279"/>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="256"/>
-      <c r="E13" s="256"/>
-      <c r="F13" s="256"/>
-      <c r="G13" s="256"/>
+      <c r="D13" s="279"/>
+      <c r="E13" s="279"/>
+      <c r="F13" s="279"/>
+      <c r="G13" s="279"/>
     </row>
     <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="256"/>
-      <c r="E14" s="256"/>
-      <c r="F14" s="256"/>
-      <c r="G14" s="256"/>
+      <c r="D14" s="279"/>
+      <c r="E14" s="279"/>
+      <c r="F14" s="279"/>
+      <c r="G14" s="279"/>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="256"/>
-      <c r="E15" s="256"/>
-      <c r="F15" s="256"/>
-      <c r="G15" s="256"/>
+      <c r="D15" s="279"/>
+      <c r="E15" s="279"/>
+      <c r="F15" s="279"/>
+      <c r="G15" s="279"/>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="256"/>
-      <c r="E16" s="256"/>
-      <c r="F16" s="256"/>
-      <c r="G16" s="256"/>
+      <c r="D16" s="279"/>
+      <c r="E16" s="279"/>
+      <c r="F16" s="279"/>
+      <c r="G16" s="279"/>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D17" s="256"/>
-      <c r="E17" s="256"/>
-      <c r="F17" s="256"/>
-      <c r="G17" s="256"/>
+      <c r="D17" s="279"/>
+      <c r="E17" s="279"/>
+      <c r="F17" s="279"/>
+      <c r="G17" s="279"/>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D18" s="256"/>
-      <c r="E18" s="256"/>
-      <c r="F18" s="256"/>
-      <c r="G18" s="256"/>
+      <c r="D18" s="279"/>
+      <c r="E18" s="279"/>
+      <c r="F18" s="279"/>
+      <c r="G18" s="279"/>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D19" s="256"/>
-      <c r="E19" s="256"/>
-      <c r="F19" s="256"/>
-      <c r="G19" s="256"/>
+      <c r="D19" s="279"/>
+      <c r="E19" s="279"/>
+      <c r="F19" s="279"/>
+      <c r="G19" s="279"/>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D24" s="256" t="s">
+      <c r="D24" s="279" t="s">
         <v>660</v>
       </c>
-      <c r="E24" s="256"/>
-      <c r="F24" s="256"/>
-      <c r="G24" s="256"/>
+      <c r="E24" s="279"/>
+      <c r="F24" s="279"/>
+      <c r="G24" s="279"/>
     </row>
     <row r="25" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D25" s="256"/>
-      <c r="E25" s="256"/>
-      <c r="F25" s="256"/>
-      <c r="G25" s="256"/>
+      <c r="D25" s="279"/>
+      <c r="E25" s="279"/>
+      <c r="F25" s="279"/>
+      <c r="G25" s="279"/>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D26" s="256"/>
-      <c r="E26" s="256"/>
-      <c r="F26" s="256"/>
-      <c r="G26" s="256"/>
+      <c r="D26" s="279"/>
+      <c r="E26" s="279"/>
+      <c r="F26" s="279"/>
+      <c r="G26" s="279"/>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D27" s="256"/>
-      <c r="E27" s="256"/>
-      <c r="F27" s="256"/>
-      <c r="G27" s="256"/>
+      <c r="D27" s="279"/>
+      <c r="E27" s="279"/>
+      <c r="F27" s="279"/>
+      <c r="G27" s="279"/>
     </row>
     <row r="28" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D28" s="256"/>
-      <c r="E28" s="256"/>
-      <c r="F28" s="256"/>
-      <c r="G28" s="256"/>
+      <c r="D28" s="279"/>
+      <c r="E28" s="279"/>
+      <c r="F28" s="279"/>
+      <c r="G28" s="279"/>
     </row>
     <row r="29" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D29" s="256"/>
-      <c r="E29" s="256"/>
-      <c r="F29" s="256"/>
-      <c r="G29" s="256"/>
+      <c r="D29" s="279"/>
+      <c r="E29" s="279"/>
+      <c r="F29" s="279"/>
+      <c r="G29" s="279"/>
     </row>
     <row r="30" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D30" s="256"/>
-      <c r="E30" s="256"/>
-      <c r="F30" s="256"/>
-      <c r="G30" s="256"/>
+      <c r="D30" s="279"/>
+      <c r="E30" s="279"/>
+      <c r="F30" s="279"/>
+      <c r="G30" s="279"/>
     </row>
     <row r="31" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D31" s="256"/>
-      <c r="E31" s="256"/>
-      <c r="F31" s="256"/>
-      <c r="G31" s="256"/>
+      <c r="D31" s="279"/>
+      <c r="E31" s="279"/>
+      <c r="F31" s="279"/>
+      <c r="G31" s="279"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>